<commit_message>
Add black border to each piece face
</commit_message>
<xml_diff>
--- a/CubeDetails.xlsx
+++ b/CubeDetails.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1 (3)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="68">
   <si>
     <t>Y</t>
   </si>
@@ -98,6 +99,138 @@
   </si>
   <si>
     <t>White</t>
+  </si>
+  <si>
+    <t>x,</t>
+  </si>
+  <si>
+    <t>DarkOrange</t>
+  </si>
+  <si>
+    <t>0.6,0.6,0.6</t>
+  </si>
+  <si>
+    <t>Piece</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>-0.5,0.6,0.6</t>
+  </si>
+  <si>
+    <t>Top Front</t>
+  </si>
+  <si>
+    <t>-1.6,0.6,0.6</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>0.6,0.6,-0.5</t>
+  </si>
+  <si>
+    <t>-0.5,0.6,-0.5</t>
+  </si>
+  <si>
+    <t>Top Middle</t>
+  </si>
+  <si>
+    <t>-1.6,0.6,-0.5</t>
+  </si>
+  <si>
+    <t>DarkGreen</t>
+  </si>
+  <si>
+    <t>0.6,0.6,-1.6</t>
+  </si>
+  <si>
+    <t>-0.5,0.6,-1.6</t>
+  </si>
+  <si>
+    <t>Top Back</t>
+  </si>
+  <si>
+    <t>-1.6,0.6,-1.6</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>0.6,-0.5,0.6</t>
+  </si>
+  <si>
+    <t>-0.5,-0.5,0.6</t>
+  </si>
+  <si>
+    <t>Front Middle</t>
+  </si>
+  <si>
+    <t>-1.6,-0.5,0.6</t>
+  </si>
+  <si>
+    <t>Mddle</t>
+  </si>
+  <si>
+    <t>0.6,-0.5,-0.5</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>-1.6,-0.5,-0.5</t>
+  </si>
+  <si>
+    <t>0.6,-0.5,-1.6</t>
+  </si>
+  <si>
+    <t>-0.5,-0.5,-1.6</t>
+  </si>
+  <si>
+    <t>Back Middle</t>
+  </si>
+  <si>
+    <t>-1.6,-0.5,-1.6</t>
+  </si>
+  <si>
+    <t>0.6,-1.6,0.6</t>
+  </si>
+  <si>
+    <t>-0.5,-1.6,0.6</t>
+  </si>
+  <si>
+    <t>Bottom Front</t>
+  </si>
+  <si>
+    <t>-1.6,-1.6,0.6</t>
+  </si>
+  <si>
+    <t>0.6,-1.6,-0.5</t>
+  </si>
+  <si>
+    <t>-0.5,-1.6,-0.5</t>
+  </si>
+  <si>
+    <t>Bottom Middle</t>
+  </si>
+  <si>
+    <t>-1.6,-1.6,-0.5</t>
+  </si>
+  <si>
+    <t>0.6,-1.6,-1.6</t>
+  </si>
+  <si>
+    <t>-0.5,-1.6,-1.6</t>
+  </si>
+  <si>
+    <t>Bottom Back</t>
+  </si>
+  <si>
+    <t>-1.6,-1.6,-1.6</t>
+  </si>
+  <si>
+    <t>X, Y, Z</t>
   </si>
 </sst>
 </file>
@@ -454,7 +587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
@@ -1421,4 +1554,751 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="9" width="15" customWidth="1"/>
+    <col min="10" max="14" width="5.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
+        <v>28</v>
+      </c>
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="I17" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" t="s">
+        <v>8</v>
+      </c>
+      <c r="O19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" t="s">
+        <v>6</v>
+      </c>
+      <c r="L21" t="s">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23" t="s">
+        <v>6</v>
+      </c>
+      <c r="L23" t="s">
+        <v>28</v>
+      </c>
+      <c r="M23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
+        <v>6</v>
+      </c>
+      <c r="L25" t="s">
+        <v>13</v>
+      </c>
+      <c r="M25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>23</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Starting change to new DL code
</commit_message>
<xml_diff>
--- a/CubeDetails.xlsx
+++ b/CubeDetails.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1 (3)" sheetId="4" r:id="rId4"/>
+    <sheet name="FaceClass" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="80">
   <si>
     <t>Y</t>
   </si>
@@ -231,6 +232,42 @@
   </si>
   <si>
     <t>X, Y, Z</t>
+  </si>
+  <si>
+    <t>Spin</t>
+  </si>
+  <si>
+    <t>Coordinates</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>D face</t>
+  </si>
+  <si>
+    <t>U face</t>
+  </si>
+  <si>
+    <t>Lface</t>
+  </si>
+  <si>
+    <t>B face</t>
+  </si>
+  <si>
+    <t>R face</t>
+  </si>
+  <si>
+    <t>F face</t>
   </si>
 </sst>
 </file>
@@ -246,17 +283,142 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -266,10 +428,74 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1560,7 +1786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2301,4 +2527,1666 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BD37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO29" sqref="AO29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="55" width="3.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B1" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="T1" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC1" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="AL1" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU1" s="57" t="s">
+        <v>74</v>
+      </c>
+      <c r="BD1" s="57"/>
+    </row>
+    <row r="2" spans="1:56" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="61">
+        <v>0</v>
+      </c>
+      <c r="C2" s="60">
+        <v>1</v>
+      </c>
+      <c r="D2" s="60">
+        <v>2</v>
+      </c>
+      <c r="E2" s="60">
+        <v>3</v>
+      </c>
+      <c r="F2" s="60">
+        <v>4</v>
+      </c>
+      <c r="G2" s="60">
+        <v>5</v>
+      </c>
+      <c r="H2" s="60">
+        <v>6</v>
+      </c>
+      <c r="I2" s="60">
+        <v>7</v>
+      </c>
+      <c r="J2" s="60">
+        <v>8</v>
+      </c>
+      <c r="K2" s="61">
+        <v>9</v>
+      </c>
+      <c r="L2" s="60">
+        <v>10</v>
+      </c>
+      <c r="M2" s="60">
+        <v>11</v>
+      </c>
+      <c r="N2" s="60">
+        <v>12</v>
+      </c>
+      <c r="O2" s="60">
+        <v>13</v>
+      </c>
+      <c r="P2" s="60">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="60">
+        <v>15</v>
+      </c>
+      <c r="R2" s="60">
+        <v>16</v>
+      </c>
+      <c r="S2" s="60">
+        <v>17</v>
+      </c>
+      <c r="T2" s="61">
+        <v>18</v>
+      </c>
+      <c r="U2" s="60">
+        <v>19</v>
+      </c>
+      <c r="V2" s="60">
+        <v>20</v>
+      </c>
+      <c r="W2" s="60">
+        <v>21</v>
+      </c>
+      <c r="X2" s="60">
+        <v>22</v>
+      </c>
+      <c r="Y2" s="60">
+        <v>23</v>
+      </c>
+      <c r="Z2" s="60">
+        <v>24</v>
+      </c>
+      <c r="AA2" s="60">
+        <v>25</v>
+      </c>
+      <c r="AB2" s="60">
+        <v>26</v>
+      </c>
+      <c r="AC2" s="61">
+        <v>27</v>
+      </c>
+      <c r="AD2" s="60">
+        <v>28</v>
+      </c>
+      <c r="AE2" s="60">
+        <v>29</v>
+      </c>
+      <c r="AF2" s="60">
+        <v>30</v>
+      </c>
+      <c r="AG2" s="60">
+        <v>31</v>
+      </c>
+      <c r="AH2" s="60">
+        <v>32</v>
+      </c>
+      <c r="AI2" s="60">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="60">
+        <v>34</v>
+      </c>
+      <c r="AK2" s="60">
+        <v>35</v>
+      </c>
+      <c r="AL2" s="61">
+        <v>36</v>
+      </c>
+      <c r="AM2" s="60">
+        <v>37</v>
+      </c>
+      <c r="AN2" s="60">
+        <v>38</v>
+      </c>
+      <c r="AO2" s="60">
+        <v>39</v>
+      </c>
+      <c r="AP2" s="60">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="60">
+        <v>41</v>
+      </c>
+      <c r="AR2" s="60">
+        <v>42</v>
+      </c>
+      <c r="AS2" s="60">
+        <v>43</v>
+      </c>
+      <c r="AT2" s="60">
+        <v>44</v>
+      </c>
+      <c r="AU2" s="61">
+        <v>45</v>
+      </c>
+      <c r="AV2" s="60">
+        <v>46</v>
+      </c>
+      <c r="AW2" s="60">
+        <v>47</v>
+      </c>
+      <c r="AX2" s="60">
+        <v>48</v>
+      </c>
+      <c r="AY2" s="60">
+        <v>49</v>
+      </c>
+      <c r="AZ2" s="60">
+        <v>50</v>
+      </c>
+      <c r="BA2" s="60">
+        <v>51</v>
+      </c>
+      <c r="BB2" s="60">
+        <v>52</v>
+      </c>
+      <c r="BC2" s="60">
+        <v>53</v>
+      </c>
+      <c r="BD2" s="61"/>
+    </row>
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="U3" t="s">
+        <v>71</v>
+      </c>
+      <c r="V3" t="s">
+        <v>71</v>
+      </c>
+      <c r="W3" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC3" s="57" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AL3" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AU3" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="57"/>
+    </row>
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="T4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AL4" s="57"/>
+      <c r="AU4" s="57"/>
+      <c r="BD4" s="57"/>
+    </row>
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="57">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>27</v>
+      </c>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="57">
+        <v>-9</v>
+      </c>
+      <c r="L5">
+        <v>-9</v>
+      </c>
+      <c r="M5">
+        <v>-9</v>
+      </c>
+      <c r="N5" s="58"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="57">
+        <v>-9</v>
+      </c>
+      <c r="U5">
+        <v>-9</v>
+      </c>
+      <c r="V5">
+        <v>-9</v>
+      </c>
+      <c r="W5" s="58"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="58"/>
+      <c r="AC5" s="57">
+        <v>-9</v>
+      </c>
+      <c r="AD5">
+        <v>-9</v>
+      </c>
+      <c r="AE5">
+        <v>-9</v>
+      </c>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="58"/>
+      <c r="AJ5" s="58"/>
+      <c r="AK5" s="58"/>
+      <c r="AL5" s="57">
+        <v>2</v>
+      </c>
+      <c r="AM5">
+        <v>4</v>
+      </c>
+      <c r="AN5">
+        <v>6</v>
+      </c>
+      <c r="AO5">
+        <v>-2</v>
+      </c>
+      <c r="AP5" s="58"/>
+      <c r="AQ5">
+        <v>2</v>
+      </c>
+      <c r="AR5">
+        <v>-6</v>
+      </c>
+      <c r="AS5">
+        <v>-4</v>
+      </c>
+      <c r="AT5">
+        <v>-2</v>
+      </c>
+      <c r="AU5" s="59"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="58"/>
+      <c r="AX5" s="58"/>
+      <c r="AY5" s="58"/>
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="58"/>
+      <c r="BC5" s="58"/>
+      <c r="BD5" s="57"/>
+    </row>
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="T6" s="57"/>
+      <c r="AC6" s="57"/>
+      <c r="AL6" s="57"/>
+      <c r="AU6" s="57"/>
+      <c r="BD6" s="57"/>
+    </row>
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="57">
+        <v>45</v>
+      </c>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7">
+        <v>45</v>
+      </c>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7">
+        <v>45</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="58"/>
+      <c r="V7">
+        <v>22</v>
+      </c>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7">
+        <v>16</v>
+      </c>
+      <c r="Z7" s="58"/>
+      <c r="AA7" s="58"/>
+      <c r="AB7">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="57">
+        <v>2</v>
+      </c>
+      <c r="AD7">
+        <v>4</v>
+      </c>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+      <c r="AF7">
+        <v>-2</v>
+      </c>
+      <c r="AG7" s="58"/>
+      <c r="AH7">
+        <v>2</v>
+      </c>
+      <c r="AI7">
+        <v>-6</v>
+      </c>
+      <c r="AJ7">
+        <v>-4</v>
+      </c>
+      <c r="AK7">
+        <v>-2</v>
+      </c>
+      <c r="AL7" s="57">
+        <v>-36</v>
+      </c>
+      <c r="AM7" s="58"/>
+      <c r="AN7" s="58"/>
+      <c r="AO7">
+        <v>-36</v>
+      </c>
+      <c r="AP7" s="58"/>
+      <c r="AQ7" s="58"/>
+      <c r="AR7">
+        <v>-36</v>
+      </c>
+      <c r="AS7" s="58"/>
+      <c r="AT7" s="58"/>
+      <c r="AU7" s="57">
+        <v>-19</v>
+      </c>
+      <c r="AV7" s="58"/>
+      <c r="AW7" s="58"/>
+      <c r="AX7">
+        <v>-25</v>
+      </c>
+      <c r="AY7" s="58"/>
+      <c r="AZ7" s="58"/>
+      <c r="BA7">
+        <v>-31</v>
+      </c>
+      <c r="BB7" s="58"/>
+      <c r="BC7" s="58"/>
+      <c r="BD7" s="57"/>
+    </row>
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B8" s="57"/>
+      <c r="K8" s="57"/>
+      <c r="T8" s="57"/>
+      <c r="AC8" s="57"/>
+      <c r="AL8" s="57"/>
+      <c r="AU8" s="57"/>
+      <c r="BD8" s="57"/>
+    </row>
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="57">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>-2</v>
+      </c>
+      <c r="F9" s="58"/>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>-6</v>
+      </c>
+      <c r="I9">
+        <v>-4</v>
+      </c>
+      <c r="J9">
+        <v>-2</v>
+      </c>
+      <c r="K9" s="57">
+        <v>38</v>
+      </c>
+      <c r="L9" s="58"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="52">
+        <v>34</v>
+      </c>
+      <c r="O9" s="58"/>
+      <c r="P9" s="58"/>
+      <c r="Q9" s="11">
+        <v>30</v>
+      </c>
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="58"/>
+      <c r="X9" s="58"/>
+      <c r="Y9" s="58"/>
+      <c r="Z9" s="58"/>
+      <c r="AA9" s="58"/>
+      <c r="AB9" s="58"/>
+      <c r="AC9" s="59"/>
+      <c r="AD9" s="58"/>
+      <c r="AE9">
+        <v>16</v>
+      </c>
+      <c r="AF9" s="58"/>
+      <c r="AG9" s="58"/>
+      <c r="AH9">
+        <v>18</v>
+      </c>
+      <c r="AI9" s="58"/>
+      <c r="AJ9" s="58"/>
+      <c r="AK9">
+        <v>12</v>
+      </c>
+      <c r="AL9" s="59"/>
+      <c r="AM9" s="58"/>
+      <c r="AN9" s="58"/>
+      <c r="AO9" s="58"/>
+      <c r="AP9" s="58"/>
+      <c r="AQ9" s="58"/>
+      <c r="AR9">
+        <v>-7</v>
+      </c>
+      <c r="AS9" s="11">
+        <v>-11</v>
+      </c>
+      <c r="AT9" s="11">
+        <v>-15</v>
+      </c>
+      <c r="AU9" s="57">
+        <v>-16</v>
+      </c>
+      <c r="AV9" s="58"/>
+      <c r="AW9" s="58"/>
+      <c r="AX9" s="52">
+        <v>-16</v>
+      </c>
+      <c r="AY9" s="58"/>
+      <c r="AZ9" s="58"/>
+      <c r="BA9">
+        <v>-16</v>
+      </c>
+      <c r="BB9" s="58"/>
+      <c r="BC9" s="58"/>
+      <c r="BD9" s="57"/>
+    </row>
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B10" s="57"/>
+      <c r="K10" s="57"/>
+      <c r="T10" s="57"/>
+      <c r="AC10" s="57"/>
+      <c r="AL10" s="57"/>
+      <c r="AU10" s="57"/>
+      <c r="BD10" s="57"/>
+    </row>
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="58"/>
+      <c r="D11">
+        <v>36</v>
+      </c>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
+      <c r="G11">
+        <v>36</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="58"/>
+      <c r="J11">
+        <v>36</v>
+      </c>
+      <c r="K11" s="57">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>-2</v>
+      </c>
+      <c r="O11" s="58"/>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>-6</v>
+      </c>
+      <c r="R11">
+        <v>-4</v>
+      </c>
+      <c r="S11">
+        <v>-2</v>
+      </c>
+      <c r="T11" s="57">
+        <v>35</v>
+      </c>
+      <c r="U11" s="58"/>
+      <c r="V11" s="58"/>
+      <c r="W11">
+        <v>29</v>
+      </c>
+      <c r="X11" s="58"/>
+      <c r="Y11" s="58"/>
+      <c r="Z11">
+        <v>23</v>
+      </c>
+      <c r="AA11" s="58"/>
+      <c r="AB11" s="58"/>
+      <c r="AC11" s="59"/>
+      <c r="AD11" s="58"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="58"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="58"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="59"/>
+      <c r="AM11" s="58"/>
+      <c r="AN11">
+        <v>-12</v>
+      </c>
+      <c r="AO11" s="58"/>
+      <c r="AP11" s="58"/>
+      <c r="AQ11">
+        <v>-18</v>
+      </c>
+      <c r="AR11" s="58"/>
+      <c r="AS11" s="58"/>
+      <c r="AT11">
+        <v>-24</v>
+      </c>
+      <c r="AU11" s="57">
+        <v>-45</v>
+      </c>
+      <c r="AV11" s="58"/>
+      <c r="AW11" s="58"/>
+      <c r="AX11">
+        <v>-45</v>
+      </c>
+      <c r="AY11" s="58"/>
+      <c r="AZ11" s="58"/>
+      <c r="BA11">
+        <v>-45</v>
+      </c>
+      <c r="BB11" s="58"/>
+      <c r="BC11" s="58"/>
+      <c r="BD11" s="57"/>
+    </row>
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B12" s="57"/>
+      <c r="K12" s="57"/>
+      <c r="T12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AL12" s="57"/>
+      <c r="AU12" s="57"/>
+      <c r="BD12" s="57"/>
+    </row>
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="59"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="58"/>
+      <c r="M13">
+        <v>25</v>
+      </c>
+      <c r="N13" s="58"/>
+      <c r="O13" s="58"/>
+      <c r="P13">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="58"/>
+      <c r="S13">
+        <v>21</v>
+      </c>
+      <c r="T13" s="57">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>4</v>
+      </c>
+      <c r="V13">
+        <v>6</v>
+      </c>
+      <c r="W13">
+        <v>-2</v>
+      </c>
+      <c r="X13" s="58"/>
+      <c r="Y13">
+        <v>2</v>
+      </c>
+      <c r="Z13">
+        <v>-6</v>
+      </c>
+      <c r="AA13">
+        <v>-4</v>
+      </c>
+      <c r="AB13">
+        <v>-2</v>
+      </c>
+      <c r="AC13" s="57">
+        <v>26</v>
+      </c>
+      <c r="AD13" s="58"/>
+      <c r="AE13" s="58"/>
+      <c r="AF13" s="52">
+        <v>22</v>
+      </c>
+      <c r="AG13" s="58"/>
+      <c r="AH13" s="58"/>
+      <c r="AI13" s="11">
+        <v>18</v>
+      </c>
+      <c r="AJ13" s="58"/>
+      <c r="AK13" s="58"/>
+      <c r="AL13" s="57">
+        <v>-3</v>
+      </c>
+      <c r="AM13">
+        <v>-7</v>
+      </c>
+      <c r="AN13">
+        <v>-11</v>
+      </c>
+      <c r="AO13" s="58"/>
+      <c r="AP13" s="58"/>
+      <c r="AQ13" s="58"/>
+      <c r="AR13" s="58"/>
+      <c r="AS13" s="58"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="59"/>
+      <c r="AV13" s="58"/>
+      <c r="AW13" s="58"/>
+      <c r="AX13" s="58"/>
+      <c r="AY13" s="58"/>
+      <c r="AZ13" s="58"/>
+      <c r="BA13">
+        <v>-34</v>
+      </c>
+      <c r="BB13">
+        <v>-38</v>
+      </c>
+      <c r="BC13">
+        <v>-42</v>
+      </c>
+      <c r="BD13" s="57"/>
+    </row>
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B14" s="57"/>
+      <c r="K14" s="57"/>
+      <c r="T14" s="57"/>
+      <c r="AC14" s="57"/>
+      <c r="AL14" s="57"/>
+      <c r="AU14" s="57"/>
+      <c r="BD14" s="57"/>
+    </row>
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="58"/>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>9</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15" s="59"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="58"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15">
+        <v>9</v>
+      </c>
+      <c r="R15">
+        <v>9</v>
+      </c>
+      <c r="S15">
+        <v>9</v>
+      </c>
+      <c r="T15" s="59"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="58"/>
+      <c r="W15" s="58"/>
+      <c r="X15" s="58"/>
+      <c r="Y15" s="58"/>
+      <c r="Z15">
+        <v>9</v>
+      </c>
+      <c r="AA15">
+        <v>9</v>
+      </c>
+      <c r="AB15">
+        <v>9</v>
+      </c>
+      <c r="AC15" s="59"/>
+      <c r="AD15" s="58"/>
+      <c r="AE15" s="58"/>
+      <c r="AF15" s="58"/>
+      <c r="AG15" s="58"/>
+      <c r="AH15" s="58"/>
+      <c r="AI15">
+        <v>-27</v>
+      </c>
+      <c r="AJ15">
+        <v>-27</v>
+      </c>
+      <c r="AK15">
+        <v>-29</v>
+      </c>
+      <c r="AL15" s="59"/>
+      <c r="AM15" s="58"/>
+      <c r="AN15" s="58"/>
+      <c r="AO15" s="58"/>
+      <c r="AP15" s="58"/>
+      <c r="AQ15" s="58"/>
+      <c r="AR15" s="58"/>
+      <c r="AS15" s="58"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="57">
+        <v>2</v>
+      </c>
+      <c r="AV15">
+        <v>4</v>
+      </c>
+      <c r="AW15">
+        <v>6</v>
+      </c>
+      <c r="AX15">
+        <v>-2</v>
+      </c>
+      <c r="AY15" s="58"/>
+      <c r="AZ15">
+        <v>2</v>
+      </c>
+      <c r="BA15">
+        <v>-6</v>
+      </c>
+      <c r="BB15">
+        <v>-4</v>
+      </c>
+      <c r="BC15">
+        <v>-2</v>
+      </c>
+      <c r="BD15" s="57"/>
+    </row>
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B16" s="57"/>
+      <c r="K16" s="57"/>
+      <c r="T16" s="57"/>
+      <c r="AC16" s="57"/>
+      <c r="AL16" s="57"/>
+      <c r="AU16" s="57"/>
+      <c r="BD16" s="57"/>
+    </row>
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="57">
+        <v>27</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>27</v>
+      </c>
+      <c r="E17">
+        <v>27</v>
+      </c>
+      <c r="F17">
+        <v>27</v>
+      </c>
+      <c r="G17">
+        <v>27</v>
+      </c>
+      <c r="H17">
+        <v>27</v>
+      </c>
+      <c r="I17">
+        <v>27</v>
+      </c>
+      <c r="J17">
+        <v>27</v>
+      </c>
+      <c r="K17" s="57">
+        <v>-9</v>
+      </c>
+      <c r="L17">
+        <v>-9</v>
+      </c>
+      <c r="M17">
+        <v>-9</v>
+      </c>
+      <c r="N17">
+        <v>-9</v>
+      </c>
+      <c r="O17">
+        <v>-9</v>
+      </c>
+      <c r="P17">
+        <v>-9</v>
+      </c>
+      <c r="Q17">
+        <v>-9</v>
+      </c>
+      <c r="R17">
+        <v>-9</v>
+      </c>
+      <c r="S17">
+        <v>-9</v>
+      </c>
+      <c r="T17" s="57">
+        <v>-9</v>
+      </c>
+      <c r="U17">
+        <v>-9</v>
+      </c>
+      <c r="V17">
+        <v>-9</v>
+      </c>
+      <c r="W17">
+        <v>-9</v>
+      </c>
+      <c r="X17">
+        <v>-9</v>
+      </c>
+      <c r="Y17">
+        <v>-9</v>
+      </c>
+      <c r="Z17">
+        <v>-9</v>
+      </c>
+      <c r="AA17">
+        <v>-9</v>
+      </c>
+      <c r="AB17">
+        <v>-9</v>
+      </c>
+      <c r="AC17" s="57">
+        <v>-9</v>
+      </c>
+      <c r="AD17">
+        <v>-9</v>
+      </c>
+      <c r="AE17">
+        <v>-9</v>
+      </c>
+      <c r="AF17">
+        <v>-9</v>
+      </c>
+      <c r="AG17">
+        <v>-9</v>
+      </c>
+      <c r="AH17">
+        <v>-9</v>
+      </c>
+      <c r="AI17">
+        <v>-9</v>
+      </c>
+      <c r="AJ17">
+        <v>-9</v>
+      </c>
+      <c r="AK17">
+        <v>-9</v>
+      </c>
+      <c r="AL17" s="57">
+        <v>2</v>
+      </c>
+      <c r="AM17">
+        <v>4</v>
+      </c>
+      <c r="AN17">
+        <v>6</v>
+      </c>
+      <c r="AO17">
+        <v>-2</v>
+      </c>
+      <c r="AP17" s="58"/>
+      <c r="AQ17">
+        <v>2</v>
+      </c>
+      <c r="AR17">
+        <v>-6</v>
+      </c>
+      <c r="AS17">
+        <v>-4</v>
+      </c>
+      <c r="AT17">
+        <v>-2</v>
+      </c>
+      <c r="AU17" s="57">
+        <v>6</v>
+      </c>
+      <c r="AV17" s="52">
+        <v>2</v>
+      </c>
+      <c r="AW17" s="52">
+        <v>-2</v>
+      </c>
+      <c r="AX17" s="52">
+        <v>4</v>
+      </c>
+      <c r="AY17" s="58"/>
+      <c r="AZ17" s="52">
+        <v>-4</v>
+      </c>
+      <c r="BA17" s="52">
+        <v>2</v>
+      </c>
+      <c r="BB17" s="52">
+        <v>-2</v>
+      </c>
+      <c r="BC17" s="52">
+        <v>-6</v>
+      </c>
+      <c r="BD17" s="57"/>
+    </row>
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="T18" s="57"/>
+      <c r="AC18" s="57"/>
+      <c r="AL18" s="57"/>
+      <c r="AU18" s="57"/>
+      <c r="BD18" s="57"/>
+    </row>
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="57">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>36</v>
+      </c>
+      <c r="E19">
+        <v>36</v>
+      </c>
+      <c r="F19">
+        <v>36</v>
+      </c>
+      <c r="G19">
+        <v>36</v>
+      </c>
+      <c r="H19">
+        <v>36</v>
+      </c>
+      <c r="I19">
+        <v>36</v>
+      </c>
+      <c r="J19">
+        <v>36</v>
+      </c>
+      <c r="K19" s="57">
+        <v>6</v>
+      </c>
+      <c r="L19" s="52">
+        <v>2</v>
+      </c>
+      <c r="M19" s="52">
+        <v>-2</v>
+      </c>
+      <c r="N19" s="52">
+        <v>4</v>
+      </c>
+      <c r="O19" s="58"/>
+      <c r="P19" s="52">
+        <v>-4</v>
+      </c>
+      <c r="Q19" s="52">
+        <v>2</v>
+      </c>
+      <c r="R19" s="52">
+        <v>-2</v>
+      </c>
+      <c r="S19" s="52">
+        <v>-6</v>
+      </c>
+      <c r="T19" s="57">
+        <v>35</v>
+      </c>
+      <c r="U19">
+        <v>33</v>
+      </c>
+      <c r="V19">
+        <v>30</v>
+      </c>
+      <c r="W19">
+        <v>29</v>
+      </c>
+      <c r="X19">
+        <v>27</v>
+      </c>
+      <c r="Y19">
+        <v>25</v>
+      </c>
+      <c r="Z19">
+        <v>23</v>
+      </c>
+      <c r="AA19">
+        <v>21</v>
+      </c>
+      <c r="AB19">
+        <v>19</v>
+      </c>
+      <c r="AC19" s="57">
+        <v>2</v>
+      </c>
+      <c r="AD19">
+        <v>4</v>
+      </c>
+      <c r="AE19">
+        <v>6</v>
+      </c>
+      <c r="AF19">
+        <v>-2</v>
+      </c>
+      <c r="AG19" s="58"/>
+      <c r="AH19">
+        <v>2</v>
+      </c>
+      <c r="AI19">
+        <v>-6</v>
+      </c>
+      <c r="AJ19">
+        <v>-4</v>
+      </c>
+      <c r="AK19">
+        <v>-2</v>
+      </c>
+      <c r="AL19" s="57">
+        <v>-12</v>
+      </c>
+      <c r="AM19">
+        <v>-12</v>
+      </c>
+      <c r="AN19">
+        <v>-14</v>
+      </c>
+      <c r="AO19">
+        <v>-18</v>
+      </c>
+      <c r="AP19">
+        <v>-18</v>
+      </c>
+      <c r="AQ19">
+        <v>-20</v>
+      </c>
+      <c r="AR19">
+        <v>-24</v>
+      </c>
+      <c r="AS19">
+        <v>-24</v>
+      </c>
+      <c r="AT19">
+        <v>-26</v>
+      </c>
+      <c r="AU19" s="57">
+        <v>-45</v>
+      </c>
+      <c r="AV19">
+        <v>-45</v>
+      </c>
+      <c r="AW19">
+        <v>-45</v>
+      </c>
+      <c r="AX19">
+        <v>-45</v>
+      </c>
+      <c r="AY19">
+        <v>-45</v>
+      </c>
+      <c r="AZ19">
+        <v>-45</v>
+      </c>
+      <c r="BA19">
+        <v>-45</v>
+      </c>
+      <c r="BB19">
+        <v>-45</v>
+      </c>
+      <c r="BC19">
+        <v>-45</v>
+      </c>
+      <c r="BD19" s="57"/>
+    </row>
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="B20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="T20" s="57"/>
+      <c r="AC20" s="57"/>
+      <c r="AL20" s="57"/>
+      <c r="AU20" s="57"/>
+      <c r="BD20" s="57"/>
+    </row>
+    <row r="24" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F25" s="56">
+        <v>0</v>
+      </c>
+      <c r="G25" s="55">
+        <v>1</v>
+      </c>
+      <c r="H25" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="F26" s="53">
+        <v>3</v>
+      </c>
+      <c r="G26" s="52">
+        <v>4</v>
+      </c>
+      <c r="H26" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="50">
+        <v>6</v>
+      </c>
+      <c r="G27" s="49">
+        <v>7</v>
+      </c>
+      <c r="H27" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="T28" s="52">
+        <v>9</v>
+      </c>
+      <c r="U28" s="11"/>
+      <c r="V28" s="52">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>27</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>9</v>
+      </c>
+      <c r="M29">
+        <v>18</v>
+      </c>
+      <c r="P29">
+        <v>27</v>
+      </c>
+      <c r="T29" s="52">
+        <v>6</v>
+      </c>
+      <c r="U29" s="11"/>
+      <c r="V29" s="52">
+        <v>6</v>
+      </c>
+      <c r="X29">
+        <f>V29+$V$28-T29-$T$28</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="C30" s="38">
+        <v>0</v>
+      </c>
+      <c r="D30" s="37">
+        <v>1</v>
+      </c>
+      <c r="E30" s="36">
+        <v>2</v>
+      </c>
+      <c r="F30" s="47">
+        <v>0</v>
+      </c>
+      <c r="G30" s="46">
+        <v>1</v>
+      </c>
+      <c r="H30" s="45">
+        <v>2</v>
+      </c>
+      <c r="I30" s="44">
+        <v>0</v>
+      </c>
+      <c r="J30" s="43">
+        <v>1</v>
+      </c>
+      <c r="K30" s="42">
+        <v>2</v>
+      </c>
+      <c r="L30" s="41">
+        <v>0</v>
+      </c>
+      <c r="M30" s="40">
+        <v>1</v>
+      </c>
+      <c r="N30" s="39">
+        <v>2</v>
+      </c>
+      <c r="O30" s="38">
+        <v>0</v>
+      </c>
+      <c r="P30" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q30" s="36">
+        <v>2</v>
+      </c>
+      <c r="T30" s="52">
+        <v>7</v>
+      </c>
+      <c r="U30" s="11"/>
+      <c r="V30" s="52">
+        <v>7</v>
+      </c>
+      <c r="X30">
+        <f>V30+$V$28-T30-$T$28</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+      <c r="C31" s="26">
+        <v>3</v>
+      </c>
+      <c r="D31" s="25">
+        <v>4</v>
+      </c>
+      <c r="E31" s="24">
+        <v>5</v>
+      </c>
+      <c r="F31" s="35">
+        <v>3</v>
+      </c>
+      <c r="G31" s="34">
+        <v>4</v>
+      </c>
+      <c r="H31" s="33">
+        <v>5</v>
+      </c>
+      <c r="I31" s="32">
+        <v>3</v>
+      </c>
+      <c r="J31" s="31">
+        <v>4</v>
+      </c>
+      <c r="K31" s="30">
+        <v>5</v>
+      </c>
+      <c r="L31" s="29">
+        <v>3</v>
+      </c>
+      <c r="M31" s="28">
+        <v>4</v>
+      </c>
+      <c r="N31" s="27">
+        <v>5</v>
+      </c>
+      <c r="O31" s="26">
+        <v>3</v>
+      </c>
+      <c r="P31" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="24">
+        <v>5</v>
+      </c>
+      <c r="T31" s="52">
+        <v>8</v>
+      </c>
+      <c r="U31" s="11"/>
+      <c r="V31" s="52">
+        <v>8</v>
+      </c>
+      <c r="X31">
+        <f>V31+$V$28-T31-$T$28</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:56" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="14">
+        <v>6</v>
+      </c>
+      <c r="D32" s="13">
+        <v>7</v>
+      </c>
+      <c r="E32" s="12">
+        <v>8</v>
+      </c>
+      <c r="F32" s="23">
+        <v>6</v>
+      </c>
+      <c r="G32" s="22">
+        <v>7</v>
+      </c>
+      <c r="H32" s="21">
+        <v>8</v>
+      </c>
+      <c r="I32" s="20">
+        <v>6</v>
+      </c>
+      <c r="J32" s="19">
+        <v>7</v>
+      </c>
+      <c r="K32" s="18">
+        <v>8</v>
+      </c>
+      <c r="L32" s="17">
+        <v>6</v>
+      </c>
+      <c r="M32" s="16">
+        <v>7</v>
+      </c>
+      <c r="N32" s="15">
+        <v>8</v>
+      </c>
+      <c r="O32" s="14">
+        <v>6</v>
+      </c>
+      <c r="P32" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q32" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="10">
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <v>1</v>
+      </c>
+      <c r="H35" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" s="7">
+        <v>3</v>
+      </c>
+      <c r="G36" s="6">
+        <v>4</v>
+      </c>
+      <c r="H36" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="4">
+        <v>6</v>
+      </c>
+      <c r="G37" s="3">
+        <v>7</v>
+      </c>
+      <c r="H37" s="2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Solver is fully working
</commit_message>
<xml_diff>
--- a/CubeDetails.xlsx
+++ b/CubeDetails.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Public\Gitrepos\T10\Rubik2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10860" windowHeight="7965" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet1 (3)" sheetId="4" r:id="rId4"/>
     <sheet name="FaceClass" sheetId="5" r:id="rId5"/>
-    <sheet name="New Metrics" sheetId="6" r:id="rId6"/>
+    <sheet name="WhiteCross1" sheetId="7" r:id="rId6"/>
+    <sheet name="New Metrics" sheetId="6" r:id="rId7"/>
+    <sheet name="Sheet4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="107">
   <si>
     <t>Y</t>
   </si>
@@ -299,6 +301,57 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>OW</t>
+  </si>
+  <si>
+    <t>OG</t>
+  </si>
+  <si>
+    <t>OY</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>RY</t>
+  </si>
+  <si>
+    <t>SidePieces</t>
+  </si>
+  <si>
+    <t>cornerPieces</t>
+  </si>
+  <si>
+    <t>TileColor</t>
+  </si>
+  <si>
+    <t>Given a yellow cross</t>
+  </si>
+  <si>
+    <t>Possible colors of Faces 0-4 tile 1</t>
   </si>
 </sst>
 </file>
@@ -322,7 +375,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +415,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -542,6 +601,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2576,11 +2636,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ44"/>
+  <dimension ref="A1:BJ76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3110,7 +3170,7 @@
         <v>-2</v>
       </c>
       <c r="AP4" s="58">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="AQ4">
         <v>2</v>
@@ -3169,7 +3229,7 @@
       </c>
       <c r="BH4" s="52" t="str">
         <f>AL4&amp;","&amp;AM4&amp;","&amp;AN4&amp;","&amp;AO4&amp;","&amp;AP4&amp;","&amp;AQ4&amp;","&amp;AR4&amp;","&amp;AS4&amp;","&amp;AT4&amp;","</f>
-        <v>2,4,6,-2,0,2,-6,-4,-2,</v>
+        <v>2,4,6,-2,200,2,-6,-4,-2,</v>
       </c>
       <c r="BI4" s="52" t="str">
         <f>AU4&amp;","&amp;AV4&amp;","&amp;AW4&amp;","&amp;AX4&amp;","&amp;AY4&amp;","&amp;AZ4&amp;","&amp;BA4&amp;","&amp;BB4&amp;","&amp;BC4</f>
@@ -3177,7 +3237,7 @@
       </c>
       <c r="BJ4" t="str">
         <f>BD4&amp;BE4&amp;BF4&amp;BG4&amp;BH4&amp;BI4</f>
-        <v>27,27,27,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,2,4,6,-2,0,2,-6,-4,-2,0,0,0,0,0,0,0,0,0</v>
+        <v>27,27,27,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,-9,-9,-9,0,0,0,0,0,0,2,4,6,-2,200,2,-6,-4,-2,0,0,0,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="5" spans="1:62" x14ac:dyDescent="0.25">
@@ -3420,7 +3480,7 @@
         <v>-2</v>
       </c>
       <c r="F8" s="64">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="G8" s="62">
         <v>2</v>
@@ -3571,7 +3631,7 @@
       </c>
       <c r="BD8" s="63" t="str">
         <f>B8&amp;","&amp;C8&amp;","&amp;D8&amp;","&amp;E8&amp;","&amp;F8&amp;","&amp;G8&amp;","&amp;H8&amp;","&amp;I8&amp;","&amp;J8&amp;","</f>
-        <v>2,4,6,-2,0,2,-6,-4,-2,</v>
+        <v>2,4,6,-2,200,2,-6,-4,-2,</v>
       </c>
       <c r="BE8" s="65" t="str">
         <f>K8&amp;","&amp;L8&amp;","&amp;M8&amp;","&amp;N8&amp;","&amp;O8&amp;","&amp;P8&amp;","&amp;Q8&amp;","&amp;R8&amp;","&amp;S8&amp;","</f>
@@ -3595,7 +3655,7 @@
       </c>
       <c r="BJ8" s="62" t="str">
         <f>BD8&amp;BE8&amp;BF8&amp;BG8&amp;BH8&amp;BI8</f>
-        <v>2,4,6,-2,0,2,-6,-4,-2,38,0,0,34,0,0,30,0,0,0,0,0,0,0,0,0,0,0,0,0,15,0,0,11,0,0,7,0,0,0,0,0,0,-33,-31,-29,-16,-14,-12,0,0,0,0,0,0</v>
+        <v>2,4,6,-2,200,2,-6,-4,-2,38,0,0,34,0,0,30,0,0,0,0,0,0,0,0,0,0,0,0,0,15,0,0,11,0,0,7,0,0,0,0,0,0,-33,-31,-29,-16,-14,-12,0,0,0,0,0,0</v>
       </c>
     </row>
     <row r="9" spans="1:62" x14ac:dyDescent="0.25">
@@ -3656,7 +3716,7 @@
         <v>-2</v>
       </c>
       <c r="O10" s="58">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P10">
         <v>2</v>
@@ -3784,7 +3844,7 @@
       </c>
       <c r="BE10" s="52" t="str">
         <f>K10&amp;","&amp;L10&amp;","&amp;M10&amp;","&amp;N10&amp;","&amp;O10&amp;","&amp;P10&amp;","&amp;Q10&amp;","&amp;R10&amp;","&amp;S10&amp;","</f>
-        <v>2,4,6,-2,0,2,-6,-4,-2,</v>
+        <v>2,4,6,-2,200,2,-6,-4,-2,</v>
       </c>
       <c r="BF10" s="52" t="str">
         <f>T10&amp;","&amp;U10&amp;","&amp;V10&amp;","&amp;W10&amp;","&amp;X10&amp;","&amp;Y10&amp;","&amp;Z10&amp;","&amp;AA10&amp;","&amp;AB10&amp;","</f>
@@ -3804,7 +3864,7 @@
       </c>
       <c r="BJ10" t="str">
         <f>BD10&amp;BE10&amp;BF10&amp;BG10&amp;BH10&amp;BI10</f>
-        <v>0,0,36,0,0,36,0,0,36,2,4,6,-2,0,2,-6,-4,-2,35,0,0,29,0,0,23,0,0,0,0,0,0,0,0,0,0,0,0,0,-14,0,0,-20,0,0,-26,0,0,-45,0,0,-45,0,0,-45</v>
+        <v>0,0,36,0,0,36,0,0,36,2,4,6,-2,200,2,-6,-4,-2,35,0,0,29,0,0,23,0,0,0,0,0,0,0,0,0,0,0,0,0,-14,0,0,-20,0,0,-26,0,0,-45,0,0,-45,0,0,-45</v>
       </c>
     </row>
     <row r="11" spans="1:62" x14ac:dyDescent="0.25">
@@ -4729,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="AJ23">
-        <f t="shared" ref="AJ23:AJ31" si="1">W23</f>
+        <f t="shared" ref="AJ23:AJ25" si="1">W23</f>
         <v>0</v>
       </c>
       <c r="AK23">
@@ -5264,12 +5324,63 @@
         <v>-45</v>
       </c>
     </row>
-    <row r="33" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
       <c r="G33" s="11">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="V33" t="s">
+        <v>82</v>
+      </c>
+      <c r="W33">
+        <v>9</v>
+      </c>
+      <c r="X33">
+        <v>36</v>
+      </c>
+      <c r="AA33">
+        <f>X33</f>
+        <v>36</v>
+      </c>
+      <c r="AB33">
+        <v>27</v>
+      </c>
+      <c r="AE33">
+        <f>AB33</f>
+        <v>27</v>
+      </c>
+      <c r="AF33">
+        <v>45</v>
+      </c>
+      <c r="AI33">
+        <f>AF33</f>
+        <v>45</v>
+      </c>
+      <c r="AJ33">
+        <f>W33</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
       <c r="F34" s="10">
         <v>0</v>
       </c>
@@ -5279,8 +5390,58 @@
       <c r="H34" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="3:37" x14ac:dyDescent="0.25">
+      <c r="W34">
+        <v>2</v>
+      </c>
+      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
+        <f>X34-W34+X33-W33</f>
+        <v>25</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" ref="AA34:AA36" si="6">X34</f>
+        <v>0</v>
+      </c>
+      <c r="AB34">
+        <v>6</v>
+      </c>
+      <c r="AC34">
+        <f>AB34-AA34+AB33-AA33</f>
+        <v>-3</v>
+      </c>
+      <c r="AE34">
+        <f t="shared" ref="AE34:AE36" si="7">AB34</f>
+        <v>6</v>
+      </c>
+      <c r="AF34">
+        <v>8</v>
+      </c>
+      <c r="AG34">
+        <f>AF34-AE34+AF33-AE33</f>
+        <v>20</v>
+      </c>
+      <c r="AI34">
+        <f t="shared" ref="AI34:AI36" si="8">AF34</f>
+        <v>8</v>
+      </c>
+      <c r="AJ34">
+        <f t="shared" ref="AJ34:AJ36" si="9">W34</f>
+        <v>2</v>
+      </c>
+      <c r="AK34">
+        <f>AJ34-AI34+AJ33-AI33</f>
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
       <c r="F35" s="7">
         <v>3</v>
       </c>
@@ -5290,346 +5451,1607 @@
       <c r="H35" s="5">
         <v>5</v>
       </c>
-      <c r="V35" t="s">
-        <v>82</v>
-      </c>
       <c r="W35">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="X35">
-        <v>36</v>
+        <v>1</v>
+      </c>
+      <c r="Y35">
+        <f>X35-W35+X33-W33</f>
+        <v>23</v>
       </c>
       <c r="AA35">
-        <f>X35</f>
-        <v>36</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="AB35">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="AC35">
+        <f>AB35-AA35+AB33-AA33</f>
+        <v>-7</v>
       </c>
       <c r="AE35">
-        <f>AB35</f>
-        <v>27</v>
-      </c>
-      <c r="AF35">
-        <v>45</v>
-      </c>
-      <c r="AI35">
-        <f>AF35</f>
-        <v>45</v>
-      </c>
-      <c r="AJ35">
-        <f>W35</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="3:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F36" s="4">
-        <v>6</v>
-      </c>
-      <c r="G36" s="3">
-        <v>7</v>
-      </c>
-      <c r="H36" s="2">
-        <v>8</v>
-      </c>
-      <c r="W36">
-        <v>2</v>
-      </c>
-      <c r="X36">
-        <v>0</v>
-      </c>
-      <c r="Y36">
-        <f>X36-W36+X35-W35</f>
-        <v>25</v>
-      </c>
-      <c r="AA36">
-        <f t="shared" ref="AA36:AA38" si="6">X36</f>
-        <v>0</v>
-      </c>
-      <c r="AB36">
-        <v>6</v>
-      </c>
-      <c r="AC36">
-        <f>AB36-AA36+AB35-AA35</f>
-        <v>-3</v>
-      </c>
-      <c r="AE36">
-        <f t="shared" ref="AE36:AE38" si="7">AB36</f>
-        <v>6</v>
-      </c>
-      <c r="AF36">
-        <v>8</v>
-      </c>
-      <c r="AG36">
-        <f>AF36-AE36+AF35-AE35</f>
-        <v>20</v>
-      </c>
-      <c r="AI36">
-        <f t="shared" ref="AI36:AI38" si="8">AF36</f>
-        <v>8</v>
-      </c>
-      <c r="AJ36">
-        <f t="shared" ref="AJ36:AJ38" si="9">W36</f>
-        <v>2</v>
-      </c>
-      <c r="AK36">
-        <f>AJ36-AI36+AJ35-AI35</f>
-        <v>-42</v>
-      </c>
-    </row>
-    <row r="37" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="W37">
-        <v>5</v>
-      </c>
-      <c r="X37">
-        <v>1</v>
-      </c>
-      <c r="Y37">
-        <f>X37-W37+X35-W35</f>
-        <v>23</v>
-      </c>
-      <c r="AA37">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="AB37">
-        <v>3</v>
-      </c>
-      <c r="AC37">
-        <f>AB37-AA37+AB35-AA35</f>
-        <v>-7</v>
-      </c>
-      <c r="AE37">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="AF37">
-        <v>7</v>
-      </c>
-      <c r="AG37">
-        <f>AF37-AE37+AF35-AE35</f>
+      <c r="AF35">
+        <v>7</v>
+      </c>
+      <c r="AG35">
+        <f>AF35-AE35+AF33-AE33</f>
         <v>22</v>
       </c>
-      <c r="AI37">
+      <c r="AI35">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="AJ37">
+      <c r="AJ35">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="AK37">
-        <f>AJ37-AI37+AJ35-AI35</f>
+      <c r="AK35">
+        <f>AJ35-AI35+AJ33-AI33</f>
         <v>-38</v>
       </c>
     </row>
-    <row r="38" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="W38">
-        <v>8</v>
-      </c>
-      <c r="X38">
-        <v>2</v>
-      </c>
-      <c r="Y38">
-        <f>X38-W38+X35-W35</f>
+    <row r="36" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="F36" s="4">
+        <v>6</v>
+      </c>
+      <c r="G36" s="3">
+        <v>7</v>
+      </c>
+      <c r="H36" s="2">
+        <v>8</v>
+      </c>
+      <c r="W36">
+        <v>8</v>
+      </c>
+      <c r="X36">
+        <v>2</v>
+      </c>
+      <c r="Y36">
+        <f>X36-W36+X33-W33</f>
         <v>21</v>
       </c>
-      <c r="AA38">
+      <c r="AA36">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="AB38">
-        <v>0</v>
-      </c>
-      <c r="AC38">
-        <f>AB38-AA38+AB35-AA35</f>
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36">
+        <f>AB36-AA36+AB33-AA33</f>
         <v>-11</v>
       </c>
-      <c r="AE38">
+      <c r="AE36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AF38">
-        <v>6</v>
-      </c>
-      <c r="AG38">
-        <f>AF38-AE38+AF35-AE35</f>
+      <c r="AF36">
+        <v>6</v>
+      </c>
+      <c r="AG36">
+        <f>AF36-AE36+AF33-AE33</f>
         <v>24</v>
       </c>
-      <c r="AI38">
+      <c r="AI36">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="AJ38">
+      <c r="AJ36">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="AK38">
-        <f>AJ38-AI38+AJ35-AI35</f>
+      <c r="AK36">
+        <f>AJ36-AI36+AJ33-AI33</f>
         <v>-34</v>
       </c>
     </row>
-    <row r="39" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="V38" s="52"/>
+    </row>
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6">
+        <v>2</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>2</v>
+      </c>
+      <c r="O39">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>1</v>
+      </c>
+      <c r="R39">
+        <v>2</v>
+      </c>
+      <c r="S39">
+        <v>3</v>
+      </c>
+      <c r="V39" t="s">
+        <v>81</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+      <c r="X39">
+        <v>36</v>
+      </c>
+      <c r="AA39">
+        <f>X39</f>
+        <v>36</v>
+      </c>
+      <c r="AB39">
         <v>18</v>
       </c>
-    </row>
-    <row r="40" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>21</v>
+      <c r="AE39">
+        <f>AB39</f>
+        <v>18</v>
+      </c>
+      <c r="AF39">
+        <v>45</v>
+      </c>
+      <c r="AI39">
+        <f>AF39</f>
+        <v>45</v>
+      </c>
+      <c r="AJ39">
+        <f>W39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <v>4</v>
+      </c>
+      <c r="J40">
+        <v>6</v>
+      </c>
+      <c r="M40" t="s">
+        <v>8</v>
+      </c>
+      <c r="N40" t="s">
+        <v>7</v>
+      </c>
+      <c r="O40" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q40">
+        <f>C40+B40*9</f>
+        <v>0</v>
+      </c>
+      <c r="R40">
+        <f>G40+F40*9</f>
+        <v>29</v>
+      </c>
+      <c r="S40">
+        <f>J40+I40*9</f>
+        <v>42</v>
       </c>
       <c r="U40" s="11"/>
-      <c r="V40" s="52"/>
-    </row>
-    <row r="41" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>20</v>
+      <c r="W40">
+        <v>2</v>
+      </c>
+      <c r="X40">
+        <v>2</v>
+      </c>
+      <c r="Y40">
+        <f>X40-W40+X39-W39</f>
+        <v>36</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" ref="AA40:AA41" si="10">X40</f>
+        <v>2</v>
+      </c>
+      <c r="AB40">
+        <v>6</v>
+      </c>
+      <c r="AC40">
+        <f>AB40-AA40+AB39-AA39</f>
+        <v>-14</v>
+      </c>
+      <c r="AE40">
+        <f t="shared" ref="AE40:AE41" si="11">AB40</f>
+        <v>6</v>
+      </c>
+      <c r="AF40">
+        <v>2</v>
+      </c>
+      <c r="AG40">
+        <f>AF40-AE40+AF39-AE39</f>
+        <v>23</v>
+      </c>
+      <c r="AI40">
+        <f t="shared" ref="AI40:AI41" si="12">AF40</f>
+        <v>2</v>
+      </c>
+      <c r="AJ40">
+        <f t="shared" ref="AJ40:AJ41" si="13">W40</f>
+        <v>2</v>
+      </c>
+      <c r="AK40">
+        <f>AJ40-AI40+AJ39-AI39</f>
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="F41" s="6">
+        <v>4</v>
+      </c>
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="M41" t="s">
+        <v>8</v>
+      </c>
+      <c r="N41" t="s">
+        <v>68</v>
+      </c>
+      <c r="O41" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" ref="Q41:Q47" si="14">C41+B41*9</f>
+        <v>2</v>
+      </c>
+      <c r="R41">
+        <f t="shared" ref="R41:R47" si="15">G41+F41*9</f>
+        <v>44</v>
+      </c>
+      <c r="S41">
+        <f t="shared" ref="S41:S47" si="16">J41+I41*9</f>
+        <v>9</v>
       </c>
       <c r="U41" s="11"/>
-      <c r="V41" t="s">
-        <v>81</v>
-      </c>
       <c r="W41">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="X41">
+        <v>5</v>
+      </c>
+      <c r="Y41">
+        <f>X41-W41+X39-W39</f>
         <v>36</v>
       </c>
       <c r="AA41">
-        <f>X41</f>
-        <v>36</v>
-      </c>
-      <c r="AB41">
-        <v>18</v>
-      </c>
-      <c r="AE41">
-        <f>AB41</f>
-        <v>18</v>
-      </c>
-      <c r="AF41">
-        <v>45</v>
-      </c>
-      <c r="AI41">
-        <f>AF41</f>
-        <v>45</v>
-      </c>
-      <c r="AJ41">
-        <f>W41</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>19</v>
-      </c>
-      <c r="U42" s="11"/>
-      <c r="W42">
-        <v>2</v>
-      </c>
-      <c r="X42">
-        <v>2</v>
-      </c>
-      <c r="Y42">
-        <f>X42-W42+X41-W41</f>
-        <v>36</v>
-      </c>
-      <c r="AA42">
-        <f t="shared" ref="AA42:AA43" si="10">X42</f>
-        <v>2</v>
-      </c>
-      <c r="AB42">
-        <v>6</v>
-      </c>
-      <c r="AC42">
-        <f>AB42-AA42+AB41-AA41</f>
-        <v>-14</v>
-      </c>
-      <c r="AE42">
-        <f t="shared" ref="AE42:AE43" si="11">AB42</f>
-        <v>6</v>
-      </c>
-      <c r="AF42">
-        <v>2</v>
-      </c>
-      <c r="AG42">
-        <f>AF42-AE42+AF41-AE41</f>
-        <v>23</v>
-      </c>
-      <c r="AI42">
-        <f t="shared" ref="AI42:AI43" si="12">AF42</f>
-        <v>2</v>
-      </c>
-      <c r="AJ42">
-        <f t="shared" ref="AJ42:AJ43" si="13">W42</f>
-        <v>2</v>
-      </c>
-      <c r="AK42">
-        <f>AJ42-AI42+AJ41-AI41</f>
-        <v>-45</v>
-      </c>
-    </row>
-    <row r="43" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>23</v>
-      </c>
-      <c r="U43" s="11"/>
-      <c r="W43">
-        <v>5</v>
-      </c>
-      <c r="X43">
-        <v>5</v>
-      </c>
-      <c r="Y43">
-        <f>X43-W43+X41-W41</f>
-        <v>36</v>
-      </c>
-      <c r="AA43">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="AB43">
+      <c r="AB41">
         <v>3</v>
       </c>
-      <c r="AC43">
-        <f>AB43-AA43+AB41-AA41</f>
+      <c r="AC41">
+        <f>AB41-AA41+AB39-AA39</f>
         <v>-20</v>
       </c>
-      <c r="AE43">
+      <c r="AE41">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="AF43">
+      <c r="AF41">
         <v>5</v>
       </c>
-      <c r="AG43">
-        <f>AF43-AE43+AF41-AE41</f>
+      <c r="AG41">
+        <f>AF41-AE41+AF39-AE39</f>
         <v>29</v>
       </c>
-      <c r="AI43">
+      <c r="AI41">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="AJ43">
+      <c r="AJ41">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="AK43">
-        <f>AJ43-AI43+AJ41-AI41</f>
+      <c r="AK41">
+        <f>AJ41-AI41+AJ39-AI39</f>
         <v>-45</v>
       </c>
     </row>
-    <row r="44" spans="3:37" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>22</v>
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>6</v>
+      </c>
+      <c r="F42" s="6">
+        <v>5</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>8</v>
+      </c>
+      <c r="M42" t="s">
+        <v>8</v>
+      </c>
+      <c r="N42" t="s">
+        <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="14"/>
+        <v>6</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="15"/>
+        <v>45</v>
+      </c>
+      <c r="S42">
+        <f t="shared" si="16"/>
+        <v>35</v>
+      </c>
+      <c r="U42" s="11"/>
+    </row>
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>0</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="I43">
+        <v>5</v>
+      </c>
+      <c r="J43">
+        <v>2</v>
+      </c>
+      <c r="M43" t="s">
+        <v>8</v>
+      </c>
+      <c r="N43" t="s">
+        <v>70</v>
+      </c>
+      <c r="O43" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="14"/>
+        <v>8</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="S43">
+        <f t="shared" si="16"/>
+        <v>47</v>
+      </c>
+      <c r="U43" s="11"/>
+    </row>
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <v>4</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="M44" t="s">
+        <v>69</v>
+      </c>
+      <c r="N44" t="s">
+        <v>70</v>
+      </c>
+      <c r="O44" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="14"/>
+        <v>18</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="S44">
+        <f t="shared" si="16"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="M45" t="s">
+        <v>69</v>
+      </c>
+      <c r="N45" t="s">
+        <v>68</v>
+      </c>
+      <c r="O45" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="14"/>
+        <v>20</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="15"/>
+        <v>36</v>
+      </c>
+      <c r="S45">
+        <f t="shared" si="16"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>6</v>
+      </c>
+      <c r="F46">
+        <v>5</v>
+      </c>
+      <c r="G46">
+        <v>8</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>8</v>
+      </c>
+      <c r="M46" t="s">
+        <v>69</v>
+      </c>
+      <c r="N46" t="s">
+        <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="14"/>
+        <v>24</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="15"/>
+        <v>53</v>
+      </c>
+      <c r="S46">
+        <f t="shared" si="16"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>3</v>
+      </c>
+      <c r="G47">
+        <v>6</v>
+      </c>
+      <c r="I47">
+        <v>5</v>
+      </c>
+      <c r="J47">
+        <v>6</v>
+      </c>
+      <c r="M47" t="s">
+        <v>69</v>
+      </c>
+      <c r="N47" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="14"/>
+        <v>26</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="15"/>
+        <v>33</v>
+      </c>
+      <c r="S47">
+        <f t="shared" si="16"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q50" t="str">
+        <f>"ix1="&amp;Q40</f>
+        <v>ix1=0</v>
+      </c>
+      <c r="R50" t="str">
+        <f>", ix2="&amp;R40&amp;", "</f>
+        <v xml:space="preserve">, ix2=29, </v>
+      </c>
+      <c r="S50" t="str">
+        <f>"ix3="&amp;S40</f>
+        <v>ix3=42</v>
+      </c>
+      <c r="V50" t="str">
+        <f>Q50&amp;R50&amp;S50</f>
+        <v>ix1=0, ix2=29, ix3=42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q51" t="str">
+        <f t="shared" ref="Q51:Q60" si="17">"ix1="&amp;Q41</f>
+        <v>ix1=2</v>
+      </c>
+      <c r="R51" t="str">
+        <f t="shared" ref="R51:R60" si="18">", ix2="&amp;R41&amp;", "</f>
+        <v xml:space="preserve">, ix2=44, </v>
+      </c>
+      <c r="S51" t="str">
+        <f t="shared" ref="S51:S60" si="19">"ix3="&amp;S41</f>
+        <v>ix3=9</v>
+      </c>
+      <c r="V51" t="str">
+        <f t="shared" ref="V51:V60" si="20">Q51&amp;R51&amp;S51</f>
+        <v>ix1=2, ix2=44, ix3=9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="Q52" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=6</v>
+      </c>
+      <c r="R52" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=45, </v>
+      </c>
+      <c r="S52" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=35</v>
+      </c>
+      <c r="V52" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=6, ix2=45, ix3=35</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=8</v>
+      </c>
+      <c r="R53" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=15, </v>
+      </c>
+      <c r="S53" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=47</v>
+      </c>
+      <c r="V53" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=8, ix2=15, ix3=47</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>43</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>2</v>
+      </c>
+      <c r="Q54" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=18</v>
+      </c>
+      <c r="R54" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=11, </v>
+      </c>
+      <c r="S54" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=38</v>
+      </c>
+      <c r="V54" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=18, ix2=11, ix3=38</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>12</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>6</v>
+      </c>
+      <c r="Q55" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=20</v>
+      </c>
+      <c r="R55" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=36, </v>
+      </c>
+      <c r="S55" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=27</v>
+      </c>
+      <c r="V55" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=20, ix2=36, ix3=27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>92</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>46</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>8</v>
+      </c>
+      <c r="Q56" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=24</v>
+      </c>
+      <c r="R56" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=53, </v>
+      </c>
+      <c r="S56" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=17</v>
+      </c>
+      <c r="V56" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=24, ix2=53, ix3=17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57">
+        <v>3</v>
+      </c>
+      <c r="C57">
+        <v>32</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="str">
+        <f t="shared" si="17"/>
+        <v>ix1=26</v>
+      </c>
+      <c r="R57" t="str">
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">, ix2=33, </v>
+      </c>
+      <c r="S57" t="str">
+        <f t="shared" si="19"/>
+        <v>ix3=51</v>
+      </c>
+      <c r="V57" t="str">
+        <f t="shared" si="20"/>
+        <v>ix1=26, ix2=33, ix3=51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>41</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B59">
+        <v>14</v>
+      </c>
+      <c r="C59">
+        <v>21</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60">
+        <v>16</v>
+      </c>
+      <c r="C60">
+        <v>50</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61">
+        <v>19</v>
+      </c>
+      <c r="C61">
+        <v>37</v>
+      </c>
+      <c r="K61">
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>98</v>
+      </c>
+      <c r="B62">
+        <v>23</v>
+      </c>
+      <c r="C62">
+        <v>30</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+      <c r="B63">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>52</v>
+      </c>
+      <c r="K63">
+        <v>2</v>
+      </c>
+      <c r="L63">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64">
+        <v>28</v>
+      </c>
+      <c r="C64">
+        <v>39</v>
+      </c>
+      <c r="K64">
+        <v>2</v>
+      </c>
+      <c r="L64">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65">
+        <v>34</v>
+      </c>
+      <c r="C65">
+        <v>48</v>
+      </c>
+      <c r="K65">
+        <v>3</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K66" s="6">
+        <v>3</v>
+      </c>
+      <c r="L66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <v>3</v>
+      </c>
+      <c r="L67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <v>3</v>
+      </c>
+      <c r="L68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>4</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>4</v>
+      </c>
+      <c r="L70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>4</v>
+      </c>
+      <c r="L71">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K72" s="6">
+        <v>4</v>
+      </c>
+      <c r="L72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K73" s="6">
+        <v>5</v>
+      </c>
+      <c r="L73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>5</v>
+      </c>
+      <c r="L74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <v>5</v>
+      </c>
+      <c r="L75">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <v>5</v>
+      </c>
+      <c r="L76">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="K53:L76">
+    <sortCondition ref="K53:K76"/>
+    <sortCondition ref="L53:L76"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:W33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15:V25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="17" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="F3" s="56">
+        <v>0</v>
+      </c>
+      <c r="G3" s="55">
+        <v>1</v>
+      </c>
+      <c r="H3" s="54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="F4" s="53">
+        <v>3</v>
+      </c>
+      <c r="G4" s="52">
+        <v>4</v>
+      </c>
+      <c r="H4" s="51">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="50">
+        <v>6</v>
+      </c>
+      <c r="G5" s="49">
+        <v>7</v>
+      </c>
+      <c r="H5" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>27</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="M7">
+        <v>18</v>
+      </c>
+      <c r="P7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C8" s="38">
+        <v>0</v>
+      </c>
+      <c r="D8" s="37">
+        <v>1</v>
+      </c>
+      <c r="E8" s="36">
+        <v>2</v>
+      </c>
+      <c r="F8" s="47">
+        <v>0</v>
+      </c>
+      <c r="G8" s="46">
+        <v>1</v>
+      </c>
+      <c r="H8" s="45">
+        <v>2</v>
+      </c>
+      <c r="I8" s="44">
+        <v>0</v>
+      </c>
+      <c r="J8" s="43">
+        <v>1</v>
+      </c>
+      <c r="K8" s="42">
+        <v>2</v>
+      </c>
+      <c r="L8" s="41">
+        <v>0</v>
+      </c>
+      <c r="M8" s="40">
+        <v>1</v>
+      </c>
+      <c r="N8" s="39">
+        <v>2</v>
+      </c>
+      <c r="O8" s="38">
+        <v>0</v>
+      </c>
+      <c r="P8" s="37">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="26">
+        <v>3</v>
+      </c>
+      <c r="D9" s="25">
+        <v>4</v>
+      </c>
+      <c r="E9" s="24">
+        <v>5</v>
+      </c>
+      <c r="F9" s="35">
+        <v>3</v>
+      </c>
+      <c r="G9" s="34">
+        <v>4</v>
+      </c>
+      <c r="H9" s="33">
+        <v>5</v>
+      </c>
+      <c r="I9" s="32">
+        <v>3</v>
+      </c>
+      <c r="J9" s="31">
+        <v>4</v>
+      </c>
+      <c r="K9" s="30">
+        <v>5</v>
+      </c>
+      <c r="L9" s="29">
+        <v>3</v>
+      </c>
+      <c r="M9" s="28">
+        <v>4</v>
+      </c>
+      <c r="N9" s="27">
+        <v>5</v>
+      </c>
+      <c r="O9" s="26">
+        <v>3</v>
+      </c>
+      <c r="P9" s="25">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="14">
+        <v>6</v>
+      </c>
+      <c r="D10" s="13">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12">
+        <v>8</v>
+      </c>
+      <c r="F10" s="23">
+        <v>6</v>
+      </c>
+      <c r="G10" s="22">
+        <v>7</v>
+      </c>
+      <c r="H10" s="21">
+        <v>8</v>
+      </c>
+      <c r="I10" s="20">
+        <v>6</v>
+      </c>
+      <c r="J10" s="19">
+        <v>7</v>
+      </c>
+      <c r="K10" s="18">
+        <v>8</v>
+      </c>
+      <c r="L10" s="17">
+        <v>6</v>
+      </c>
+      <c r="M10" s="16">
+        <v>7</v>
+      </c>
+      <c r="N10" s="15">
+        <v>8</v>
+      </c>
+      <c r="O10" s="14">
+        <v>6</v>
+      </c>
+      <c r="P10" s="13">
+        <v>7</v>
+      </c>
+      <c r="Q10" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="F14" s="7">
+        <v>3</v>
+      </c>
+      <c r="G14" s="6">
+        <v>4</v>
+      </c>
+      <c r="H14" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="4">
+        <v>6</v>
+      </c>
+      <c r="G15" s="3">
+        <v>7</v>
+      </c>
+      <c r="H15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" t="s">
+        <v>105</v>
+      </c>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
+      <c r="V17" s="11"/>
+      <c r="W17" s="11"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>106</v>
+      </c>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
+      <c r="U18" s="11"/>
+      <c r="V18" s="11"/>
+      <c r="W18" s="11"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="G20" s="68">
+        <v>0</v>
+      </c>
+      <c r="H20" s="68">
+        <v>1</v>
+      </c>
+      <c r="I20" s="68">
+        <v>2</v>
+      </c>
+      <c r="J20" s="68">
+        <v>3</v>
+      </c>
+      <c r="R20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
+      <c r="U20" s="11"/>
+      <c r="V20" s="11"/>
+      <c r="W20" s="11"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="G21" s="68">
+        <v>0</v>
+      </c>
+      <c r="H21" s="68">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>3</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="R21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
+      <c r="U21" s="11"/>
+      <c r="V21" s="11"/>
+      <c r="W21" s="11"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="68">
+        <v>2</v>
+      </c>
+      <c r="I22" s="68">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="11"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="G23" s="68">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" s="68">
+        <v>3</v>
+      </c>
+      <c r="R23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
+      <c r="U23" s="11"/>
+      <c r="V23" s="11"/>
+      <c r="W23" s="11"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>3</v>
+      </c>
+      <c r="I24" s="68">
+        <v>1</v>
+      </c>
+      <c r="J24" s="68">
+        <v>2</v>
+      </c>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
+      <c r="U24" s="11"/>
+      <c r="V24" s="11"/>
+      <c r="W24" s="11"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="G27" s="68">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27" s="68">
+        <v>1</v>
+      </c>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+      <c r="V28" s="11"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="R29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
+      <c r="U29" s="11"/>
+      <c r="V29" s="11"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="R30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
+      <c r="U30" s="11"/>
+      <c r="V30" s="11"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="R31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
+      <c r="U31" s="11"/>
+      <c r="V31" s="11"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+    </row>
+    <row r="33" spans="18:22" x14ac:dyDescent="0.25">
+      <c r="R33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
+      <c r="U33" s="11"/>
+      <c r="V33" s="11"/>
+    </row>
+  </sheetData>
+  <sortState ref="A18:B23">
+    <sortCondition ref="B18:B23"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
@@ -6621,4 +8043,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>